<commit_message>
Getting ready to send out to collaborators
</commit_message>
<xml_diff>
--- a/spec/0.1/samples/sample/data/CATALOG_sample.xlsx
+++ b/spec/0.1/samples/sample/data/CATALOG_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="955" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Collection" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,11 +19,6 @@
     <sheet name="Projects" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -51,171 +46,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample dataset for DataCrate v.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a simple dataset for demonstration purposes it contains just one image.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DatePublished</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peter Sefton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:Creator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:ContentLocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catalina Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:RelatedLink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://dx.doi.org/10.1000/654321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:Publisher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of Technology Sydney</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:Contributor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DataCrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FILE:Filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:Creator*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">License</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATION:Affiliation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPE:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://orcid.org/0000-0002-3545-944X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sefton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pt@ptsefton.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPL1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPL1 Camera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olympus camera with Panasonic 20mm lens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://en.wikipedia.org/wiki/Olympus_PEN_E-PL1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geo&gt;GeoCoordinates&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.geonames.org/8152662/catalina-park.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://en.wikipedia.org/wiki/Catalina_Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catalina Park is a disused motor racing venue, located at Katoomba, in the Blue Mountains, New South Wales, Australia, and is recognised as an Aboriginal Place due to the long association of the local Gundungarra and Darug clans to the area.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katoomba, NSW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude: -33.7152, Longitude: 150.30119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REL:Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://uts.edu.au</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Broadway, 2007, NSW Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://creativecommons.org/licenses/by-nc-sa/3.0/au/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC BY-NC-SA 3.0 AU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attribution-NonCommercial-ShareAlike 3.0 Australia (CC BY-NC-SA 3.0 AU)
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Sample dataset for DataCrate v.01</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This is a simple dataset for demonstration purposes it contains just one image and a directory full of useless text files.</t>
+  </si>
+  <si>
+    <t>DatePublished</t>
+  </si>
+  <si>
+    <t>RELATION:Contact</t>
+  </si>
+  <si>
+    <t>Peter Sefton</t>
+  </si>
+  <si>
+    <t>RELATION:Creator</t>
+  </si>
+  <si>
+    <t>RELATION:ContentLocation</t>
+  </si>
+  <si>
+    <t>Catalina Park</t>
+  </si>
+  <si>
+    <t>RELATION:RelatedLink</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1000/654321</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>RELATION:Publisher</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
+  </si>
+  <si>
+    <t>RELATION:Contributor</t>
+  </si>
+  <si>
+    <t>DataCrate</t>
+  </si>
+  <si>
+    <t>RELATION:Keywords</t>
+  </si>
+  <si>
+    <t>Dogs, Fences, The Gully</t>
+  </si>
+  <si>
+    <t>FILE:Filename</t>
+  </si>
+  <si>
+    <t>RELATION:Creator*</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>Given Name</t>
+  </si>
+  <si>
+    <t>Family Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>RELATION:Affiliation</t>
+  </si>
+  <si>
+    <t>TYPE:</t>
+  </si>
+  <si>
+    <t>http://orcid.org/0000-0002-3545-944X</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Sefton</t>
+  </si>
+  <si>
+    <t>pt@ptsefton.com</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>EPL1</t>
+  </si>
+  <si>
+    <t>EPL1 Camera</t>
+  </si>
+  <si>
+    <t>Olympus camera with Panasonic 20mm lens</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Olympus_PEN_E-PL1</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>geo&gt;GeoCoordinates&gt;</t>
+  </si>
+  <si>
+    <t>http://www.geonames.org/8152662/catalina-park.html</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Catalina_Park</t>
+  </si>
+  <si>
+    <t>Catalina Park is a disused motor racing venue, located at Katoomba, in the Blue Mountains, New South Wales, Australia, and is recognised as an Aboriginal Place due to the long association of the local Gundungarra and Darug clans to the area.</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Katoomba, NSW</t>
+  </si>
+  <si>
+    <t>Latitude: -33.7152, Longitude: 150.30119</t>
+  </si>
+  <si>
+    <t>REL:Location</t>
+  </si>
+  <si>
+    <t>http://uts.edu.au</t>
+  </si>
+  <si>
+    <t>Broadway, 2007, NSW Australia</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-sa/3.0/au/</t>
+  </si>
+  <si>
+    <t>CC BY-NC-SA 3.0 AU</t>
+  </si>
+  <si>
+    <t>Attribution-NonCommercial-ShareAlike 3.0 Australia (CC BY-NC-SA 3.0 AU)
 This is a human-readable summary of (and not a substitute for) the license. Disclaimer.
 You are free to:
 Share — copy and redistribute the material in any medium or format
@@ -228,31 +229,31 @@
 No additional restrictions — You may not apply legal terms or technological measures that legally restrict others from doing anything the license permits.</t>
   </si>
   <si>
-    <t xml:space="preserve">DC:CREATOR*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.1000/123456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is an example publication with a dodgy DOI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScholarlyWork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/UTS-eResearch/datacrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The DataCrate project is to write the spec for DataCrate, of which this is an example.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project</t>
+    <t>DC:CREATOR*</t>
+  </si>
+  <si>
+    <t>10.1000/123456</t>
+  </si>
+  <si>
+    <t>This is an example publication with a dodgy DOI</t>
+  </si>
+  <si>
+    <t>ScholarlyWork</t>
+  </si>
+  <si>
+    <t>Funder</t>
+  </si>
+  <si>
+    <t>https://github.com/UTS-eResearch/datacrate</t>
+  </si>
+  <si>
+    <t>The DataCrate project is to write the spec for DataCrate, of which this is an example.</t>
+  </si>
+  <si>
+    <t>UTS</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -260,7 +261,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="6">
@@ -413,10 +414,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -512,6 +513,14 @@
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -545,16 +554,16 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -600,46 +609,46 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="7" t="str">
         <f aca="false">CONCATENATE(C2, " ",D2)</f>
         <v>Peter Sefton</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -683,27 +692,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +733,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -741,7 +750,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -750,36 +759,36 @@
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -822,27 +831,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -888,13 +897,13 @@
     </row>
     <row r="2" customFormat="false" ht="354.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -934,24 +943,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -995,27 +1004,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>